<commit_message>
without design & red
</commit_message>
<xml_diff>
--- a/Sources/math_11.10.2024.xlsx
+++ b/Sources/math_11.10.2024.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
-  <workbookPr defaultThemeVersion="202300"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://admortgage-my.sharepoint.com/personal/samat_dzhumagaliev_admortgage_com/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lazti\Desktop\hackathon_2025_autumn\Sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A234134D-11E6-4160-BF24-670CF841154A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="2355" windowWidth="21600" windowHeight="11295" xr2:uid="{69F9BA17-3482-4B83-AE9F-205E241B8558}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="198">
   <si>
     <t>ученик</t>
   </si>
@@ -419,221 +418,224 @@
     <t>Устинов</t>
   </si>
   <si>
+    <t>Евдокимов</t>
+  </si>
+  <si>
+    <t>Воронов</t>
+  </si>
+  <si>
+    <t>Абрамов</t>
+  </si>
+  <si>
+    <t>Карпов</t>
+  </si>
+  <si>
+    <t>Антонов</t>
+  </si>
+  <si>
+    <t>Егоров</t>
+  </si>
+  <si>
+    <t>Галкин</t>
+  </si>
+  <si>
+    <t>Щербаков</t>
+  </si>
+  <si>
+    <t>Михеев</t>
+  </si>
+  <si>
+    <t>Кошелев</t>
+  </si>
+  <si>
+    <t>Дьячков</t>
+  </si>
+  <si>
+    <t>Еремин</t>
+  </si>
+  <si>
+    <t>Тетерин</t>
+  </si>
+  <si>
+    <t>Климов</t>
+  </si>
+  <si>
+    <t>Колесников</t>
+  </si>
+  <si>
+    <t>Черкасов</t>
+  </si>
+  <si>
+    <t>Потапов</t>
+  </si>
+  <si>
+    <t>Никифоров</t>
+  </si>
+  <si>
+    <t>Комиссаров</t>
+  </si>
+  <si>
+    <t>Малышев</t>
+  </si>
+  <si>
+    <t>Лихачёв</t>
+  </si>
+  <si>
+    <t>Зуев</t>
+  </si>
+  <si>
+    <t>Русаков</t>
+  </si>
+  <si>
+    <t>Тихонов</t>
+  </si>
+  <si>
+    <t>Игнатьев</t>
+  </si>
+  <si>
+    <t>Савин</t>
+  </si>
+  <si>
+    <t>Логинов</t>
+  </si>
+  <si>
+    <t>Горшков</t>
+  </si>
+  <si>
+    <t>Князев</t>
+  </si>
+  <si>
+    <t>Афанасьев</t>
+  </si>
+  <si>
+    <t>Шилов</t>
+  </si>
+  <si>
+    <t>Константинов</t>
+  </si>
+  <si>
+    <t>Демин</t>
+  </si>
+  <si>
+    <t>Щукин</t>
+  </si>
+  <si>
+    <t>Фирсов</t>
+  </si>
+  <si>
+    <t>Дроздов</t>
+  </si>
+  <si>
+    <t>Белоусов</t>
+  </si>
+  <si>
+    <t>Березин</t>
+  </si>
+  <si>
+    <t>Голиков</t>
+  </si>
+  <si>
+    <t>Нефёдов</t>
+  </si>
+  <si>
+    <t>Старостин</t>
+  </si>
+  <si>
+    <t>Селезнёв</t>
+  </si>
+  <si>
+    <t>Панфилов</t>
+  </si>
+  <si>
+    <t>Кононов</t>
+  </si>
+  <si>
+    <t>Демьянов</t>
+  </si>
+  <si>
+    <t>Костин</t>
+  </si>
+  <si>
+    <t>Софронов</t>
+  </si>
+  <si>
+    <t>Худяков</t>
+  </si>
+  <si>
+    <t>Гребнев</t>
+  </si>
+  <si>
+    <t>Артемьев</t>
+  </si>
+  <si>
+    <t>Ушаков</t>
+  </si>
+  <si>
+    <t>Капустин</t>
+  </si>
+  <si>
+    <t>Мясников</t>
+  </si>
+  <si>
+    <t>Суслов</t>
+  </si>
+  <si>
+    <t>Дорофеев</t>
+  </si>
+  <si>
+    <t>Сазонов</t>
+  </si>
+  <si>
+    <t>Орехов</t>
+  </si>
+  <si>
+    <t>Буров</t>
+  </si>
+  <si>
+    <t>Чистяков</t>
+  </si>
+  <si>
+    <t>Некрасов</t>
+  </si>
+  <si>
+    <t>Матвеев</t>
+  </si>
+  <si>
+    <t>Брагин</t>
+  </si>
+  <si>
+    <t>Беляков</t>
+  </si>
+  <si>
+    <t>Бобылёв</t>
+  </si>
+  <si>
+    <t>Доронин</t>
+  </si>
+  <si>
+    <t>Давыдов</t>
+  </si>
+  <si>
+    <t>Краснов</t>
+  </si>
+  <si>
+    <t>Прокофьев</t>
+  </si>
+  <si>
+    <t>Наумов</t>
+  </si>
+  <si>
+    <t>ДА</t>
+  </si>
+  <si>
     <t>Вишняков</t>
-  </si>
-  <si>
-    <t>Евдокимов</t>
-  </si>
-  <si>
-    <t>Воронов</t>
-  </si>
-  <si>
-    <t>Абрамов</t>
-  </si>
-  <si>
-    <t>Карпов</t>
-  </si>
-  <si>
-    <t>Антонов</t>
-  </si>
-  <si>
-    <t>Егоров</t>
-  </si>
-  <si>
-    <t>Галкин</t>
-  </si>
-  <si>
-    <t>Щербаков</t>
-  </si>
-  <si>
-    <t>Михеев</t>
-  </si>
-  <si>
-    <t>Кошелев</t>
-  </si>
-  <si>
-    <t>Дьячков</t>
-  </si>
-  <si>
-    <t>Еремин</t>
-  </si>
-  <si>
-    <t>Тетерин</t>
-  </si>
-  <si>
-    <t>Климов</t>
-  </si>
-  <si>
-    <t>Колесников</t>
-  </si>
-  <si>
-    <t>Черкасов</t>
-  </si>
-  <si>
-    <t>Потапов</t>
-  </si>
-  <si>
-    <t>Никифоров</t>
-  </si>
-  <si>
-    <t>Комиссаров</t>
-  </si>
-  <si>
-    <t>Малышев</t>
-  </si>
-  <si>
-    <t>Лихачёв</t>
-  </si>
-  <si>
-    <t>Зуев</t>
-  </si>
-  <si>
-    <t>Русаков</t>
-  </si>
-  <si>
-    <t>Тихонов</t>
-  </si>
-  <si>
-    <t>Игнатьев</t>
-  </si>
-  <si>
-    <t>Савин</t>
-  </si>
-  <si>
-    <t>Логинов</t>
-  </si>
-  <si>
-    <t>Горшков</t>
-  </si>
-  <si>
-    <t>Князев</t>
-  </si>
-  <si>
-    <t>Афанасьев</t>
-  </si>
-  <si>
-    <t>Шилов</t>
-  </si>
-  <si>
-    <t>Константинов</t>
-  </si>
-  <si>
-    <t>Демин</t>
-  </si>
-  <si>
-    <t>Щукин</t>
-  </si>
-  <si>
-    <t>Фирсов</t>
-  </si>
-  <si>
-    <t>Дроздов</t>
-  </si>
-  <si>
-    <t>Белоусов</t>
-  </si>
-  <si>
-    <t>Березин</t>
-  </si>
-  <si>
-    <t>Голиков</t>
-  </si>
-  <si>
-    <t>Нефёдов</t>
-  </si>
-  <si>
-    <t>Старостин</t>
-  </si>
-  <si>
-    <t>Селезнёв</t>
-  </si>
-  <si>
-    <t>Панфилов</t>
-  </si>
-  <si>
-    <t>Кононов</t>
-  </si>
-  <si>
-    <t>Демьянов</t>
-  </si>
-  <si>
-    <t>Костин</t>
-  </si>
-  <si>
-    <t>Софронов</t>
-  </si>
-  <si>
-    <t>Худяков</t>
-  </si>
-  <si>
-    <t>Гребнев</t>
-  </si>
-  <si>
-    <t>Артемьев</t>
-  </si>
-  <si>
-    <t>Ушаков</t>
-  </si>
-  <si>
-    <t>Капустин</t>
-  </si>
-  <si>
-    <t>Мясников</t>
-  </si>
-  <si>
-    <t>Суслов</t>
-  </si>
-  <si>
-    <t>Дорофеев</t>
-  </si>
-  <si>
-    <t>Сазонов</t>
-  </si>
-  <si>
-    <t>Орехов</t>
-  </si>
-  <si>
-    <t>Буров</t>
-  </si>
-  <si>
-    <t>Чистяков</t>
-  </si>
-  <si>
-    <t>Некрасов</t>
-  </si>
-  <si>
-    <t>Матвеев</t>
-  </si>
-  <si>
-    <t>Брагин</t>
-  </si>
-  <si>
-    <t>Беляков</t>
-  </si>
-  <si>
-    <t>Бобылёв</t>
-  </si>
-  <si>
-    <t>Доронин</t>
-  </si>
-  <si>
-    <t>Давыдов</t>
-  </si>
-  <si>
-    <t>Краснов</t>
-  </si>
-  <si>
-    <t>Прокофьев</t>
-  </si>
-  <si>
-    <t>Наумов</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -662,7 +664,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -685,11 +687,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -701,6 +714,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1034,19 +1048,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A047D121-E511-4A53-B54A-37B3F6A8913D}">
-  <dimension ref="A1:B201"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B202"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="B130" sqref="B130"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15.6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1054,7 +1068,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="15.6">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1062,7 +1076,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="15.6">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1070,7 +1084,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="15.6">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1078,7 +1092,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="15.6">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -1086,7 +1100,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="15.6">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -1094,7 +1108,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="15.6">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -1102,7 +1116,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="15.6">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -1110,7 +1124,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="15.6">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -1118,7 +1132,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="15.6">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -1126,7 +1140,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="15.6">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -1134,7 +1148,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" ht="15.6">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
@@ -1142,7 +1156,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" ht="15.6">
       <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
@@ -1150,7 +1164,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" ht="15.6">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
@@ -1158,7 +1172,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" ht="15.6">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
@@ -1166,7 +1180,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" ht="15.6">
       <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
@@ -1174,7 +1188,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" ht="15.6">
       <c r="A17" s="2" t="s">
         <v>17</v>
       </c>
@@ -1182,7 +1196,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" ht="15.6">
       <c r="A18" s="2" t="s">
         <v>18</v>
       </c>
@@ -1190,7 +1204,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" ht="15.6">
       <c r="A19" s="2" t="s">
         <v>19</v>
       </c>
@@ -1198,7 +1212,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" ht="15.6">
       <c r="A20" s="2" t="s">
         <v>20</v>
       </c>
@@ -1206,7 +1220,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" ht="15.6">
       <c r="A21" s="2" t="s">
         <v>21</v>
       </c>
@@ -1214,7 +1228,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" ht="15.6">
       <c r="A22" s="2" t="s">
         <v>22</v>
       </c>
@@ -1222,7 +1236,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" ht="15.6">
       <c r="A23" s="2" t="s">
         <v>23</v>
       </c>
@@ -1230,7 +1244,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" ht="15.6">
       <c r="A24" s="2" t="s">
         <v>24</v>
       </c>
@@ -1238,7 +1252,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" ht="15.6">
       <c r="A25" s="2" t="s">
         <v>25</v>
       </c>
@@ -1246,7 +1260,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" ht="15.6">
       <c r="A26" s="2" t="s">
         <v>26</v>
       </c>
@@ -1254,7 +1268,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" ht="15.6">
       <c r="A27" s="2" t="s">
         <v>27</v>
       </c>
@@ -1262,7 +1276,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" ht="15.6">
       <c r="A28" s="2" t="s">
         <v>28</v>
       </c>
@@ -1270,7 +1284,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" ht="15.6">
       <c r="A29" s="2" t="s">
         <v>29</v>
       </c>
@@ -1278,7 +1292,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" ht="15.6">
       <c r="A30" s="2" t="s">
         <v>30</v>
       </c>
@@ -1286,7 +1300,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" ht="15.6">
       <c r="A31" s="2" t="s">
         <v>31</v>
       </c>
@@ -1294,7 +1308,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" ht="15.6">
       <c r="A32" s="2" t="s">
         <v>32</v>
       </c>
@@ -1302,7 +1316,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" ht="15.6">
       <c r="A33" s="2" t="s">
         <v>33</v>
       </c>
@@ -1310,7 +1324,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" ht="15.6">
       <c r="A34" s="2" t="s">
         <v>34</v>
       </c>
@@ -1318,7 +1332,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" ht="15.6">
       <c r="A35" s="2" t="s">
         <v>35</v>
       </c>
@@ -1326,7 +1340,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" ht="15.6">
       <c r="A36" s="2" t="s">
         <v>36</v>
       </c>
@@ -1334,7 +1348,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" ht="15.6">
       <c r="A37" s="2" t="s">
         <v>37</v>
       </c>
@@ -1342,7 +1356,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" ht="15.6">
       <c r="A38" s="2" t="s">
         <v>38</v>
       </c>
@@ -1350,7 +1364,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" ht="15.6">
       <c r="A39" s="2" t="s">
         <v>39</v>
       </c>
@@ -1358,7 +1372,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" ht="15.6">
       <c r="A40" s="2" t="s">
         <v>40</v>
       </c>
@@ -1366,7 +1380,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" ht="15.6">
       <c r="A41" s="2" t="s">
         <v>41</v>
       </c>
@@ -1374,7 +1388,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" ht="15.6">
       <c r="A42" s="2" t="s">
         <v>42</v>
       </c>
@@ -1382,7 +1396,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" ht="15.6">
       <c r="A43" s="2" t="s">
         <v>43</v>
       </c>
@@ -1390,7 +1404,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" ht="15.6">
       <c r="A44" s="2" t="s">
         <v>44</v>
       </c>
@@ -1398,7 +1412,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" ht="15.6">
       <c r="A45" s="2" t="s">
         <v>45</v>
       </c>
@@ -1406,7 +1420,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" ht="15.6">
       <c r="A46" s="2" t="s">
         <v>46</v>
       </c>
@@ -1414,7 +1428,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" ht="15.6">
       <c r="A47" s="2" t="s">
         <v>47</v>
       </c>
@@ -1422,7 +1436,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" ht="15.6">
       <c r="A48" s="2" t="s">
         <v>48</v>
       </c>
@@ -1430,7 +1444,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" ht="15.6">
       <c r="A49" s="2" t="s">
         <v>49</v>
       </c>
@@ -1438,7 +1452,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" ht="15.6">
       <c r="A50" s="2" t="s">
         <v>50</v>
       </c>
@@ -1446,7 +1460,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" ht="15.6">
       <c r="A51" s="2" t="s">
         <v>51</v>
       </c>
@@ -1454,7 +1468,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" ht="15.6">
       <c r="A52" s="2" t="s">
         <v>52</v>
       </c>
@@ -1462,7 +1476,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" ht="15.6">
       <c r="A53" s="2" t="s">
         <v>53</v>
       </c>
@@ -1470,7 +1484,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" ht="15.6">
       <c r="A54" s="2" t="s">
         <v>54</v>
       </c>
@@ -1478,7 +1492,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" ht="15.6">
       <c r="A55" s="2" t="s">
         <v>55</v>
       </c>
@@ -1486,7 +1500,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" ht="15.6">
       <c r="A56" s="2" t="s">
         <v>56</v>
       </c>
@@ -1494,7 +1508,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" ht="15.6">
       <c r="A57" s="2" t="s">
         <v>57</v>
       </c>
@@ -1502,7 +1516,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" ht="15.6">
       <c r="A58" s="2" t="s">
         <v>58</v>
       </c>
@@ -1510,7 +1524,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" ht="15.6">
       <c r="A59" s="2" t="s">
         <v>59</v>
       </c>
@@ -1518,7 +1532,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" ht="15.6">
       <c r="A60" s="2" t="s">
         <v>60</v>
       </c>
@@ -1526,7 +1540,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" ht="15.6">
       <c r="A61" s="2" t="s">
         <v>61</v>
       </c>
@@ -1534,7 +1548,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" ht="15.6">
       <c r="A62" s="2" t="s">
         <v>62</v>
       </c>
@@ -1542,7 +1556,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" ht="15.6">
       <c r="A63" s="2" t="s">
         <v>63</v>
       </c>
@@ -1550,7 +1564,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" ht="15.6">
       <c r="A64" s="2" t="s">
         <v>64</v>
       </c>
@@ -1558,7 +1572,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" ht="15.6">
       <c r="A65" s="2" t="s">
         <v>65</v>
       </c>
@@ -1566,7 +1580,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" ht="15.6">
       <c r="A66" s="2" t="s">
         <v>66</v>
       </c>
@@ -1574,7 +1588,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" ht="15.6">
       <c r="A67" s="2" t="s">
         <v>4</v>
       </c>
@@ -1582,7 +1596,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" ht="15.6">
       <c r="A68" s="2" t="s">
         <v>67</v>
       </c>
@@ -1590,7 +1604,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" ht="15.6">
       <c r="A69" s="2" t="s">
         <v>68</v>
       </c>
@@ -1598,7 +1612,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" ht="15.6">
       <c r="A70" s="2" t="s">
         <v>69</v>
       </c>
@@ -1606,7 +1620,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" ht="15.6">
       <c r="A71" s="2" t="s">
         <v>70</v>
       </c>
@@ -1614,7 +1628,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" ht="15.6">
       <c r="A72" s="2" t="s">
         <v>71</v>
       </c>
@@ -1622,7 +1636,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" ht="15.6">
       <c r="A73" s="2" t="s">
         <v>72</v>
       </c>
@@ -1630,7 +1644,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" ht="15.6">
       <c r="A74" s="2" t="s">
         <v>15</v>
       </c>
@@ -1638,7 +1652,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" ht="15.6">
       <c r="A75" s="2" t="s">
         <v>73</v>
       </c>
@@ -1646,7 +1660,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" ht="15.6">
       <c r="A76" s="2" t="s">
         <v>74</v>
       </c>
@@ -1654,7 +1668,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" ht="15.6">
       <c r="A77" s="2" t="s">
         <v>75</v>
       </c>
@@ -1662,7 +1676,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" ht="15.6">
       <c r="A78" s="2" t="s">
         <v>76</v>
       </c>
@@ -1670,7 +1684,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" ht="15.6">
       <c r="A79" s="2" t="s">
         <v>77</v>
       </c>
@@ -1678,7 +1692,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" ht="15.6">
       <c r="A80" s="2" t="s">
         <v>78</v>
       </c>
@@ -1686,7 +1700,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" ht="15.6">
       <c r="A81" s="2" t="s">
         <v>79</v>
       </c>
@@ -1694,7 +1708,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" ht="15.6">
       <c r="A82" s="2" t="s">
         <v>80</v>
       </c>
@@ -1702,7 +1716,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" ht="15.6">
       <c r="A83" s="2" t="s">
         <v>81</v>
       </c>
@@ -1710,7 +1724,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" ht="15.6">
       <c r="A84" s="2" t="s">
         <v>82</v>
       </c>
@@ -1718,7 +1732,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" ht="15.6">
       <c r="A85" s="2" t="s">
         <v>83</v>
       </c>
@@ -1726,7 +1740,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" ht="15.6">
       <c r="A86" s="2" t="s">
         <v>84</v>
       </c>
@@ -1734,7 +1748,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" ht="15.6">
       <c r="A87" s="2" t="s">
         <v>85</v>
       </c>
@@ -1742,7 +1756,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" ht="15.6">
       <c r="A88" s="2" t="s">
         <v>86</v>
       </c>
@@ -1750,7 +1764,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" ht="15.6">
       <c r="A89" s="2" t="s">
         <v>80</v>
       </c>
@@ -1758,7 +1772,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" ht="15.6">
       <c r="A90" s="2" t="s">
         <v>87</v>
       </c>
@@ -1766,7 +1780,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="91" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" ht="15.6">
       <c r="A91" s="2" t="s">
         <v>88</v>
       </c>
@@ -1774,7 +1788,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="92" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" ht="15.6">
       <c r="A92" s="2" t="s">
         <v>89</v>
       </c>
@@ -1782,7 +1796,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" ht="15.6">
       <c r="A93" s="2" t="s">
         <v>90</v>
       </c>
@@ -1790,7 +1804,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="94" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" ht="15.6">
       <c r="A94" s="2" t="s">
         <v>91</v>
       </c>
@@ -1798,7 +1812,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="95" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" ht="15.6">
       <c r="A95" s="2" t="s">
         <v>92</v>
       </c>
@@ -1806,7 +1820,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" ht="15.6">
       <c r="A96" s="2" t="s">
         <v>93</v>
       </c>
@@ -1814,7 +1828,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="97" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" ht="15.6">
       <c r="A97" s="2" t="s">
         <v>94</v>
       </c>
@@ -1822,7 +1836,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="98" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" ht="15.6">
       <c r="A98" s="2" t="s">
         <v>95</v>
       </c>
@@ -1830,7 +1844,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="99" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" ht="15.6">
       <c r="A99" s="2" t="s">
         <v>96</v>
       </c>
@@ -1838,7 +1852,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="100" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" ht="15.6">
       <c r="A100" s="2" t="s">
         <v>97</v>
       </c>
@@ -1846,7 +1860,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="101" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" ht="15.6">
       <c r="A101" s="2" t="s">
         <v>98</v>
       </c>
@@ -1854,7 +1868,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="102" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" ht="15.6">
       <c r="A102" s="2" t="s">
         <v>99</v>
       </c>
@@ -1862,7 +1876,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="103" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" ht="15.6">
       <c r="A103" s="2" t="s">
         <v>100</v>
       </c>
@@ -1870,7 +1884,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="104" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" ht="15.6">
       <c r="A104" s="2" t="s">
         <v>101</v>
       </c>
@@ -1878,7 +1892,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="105" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" ht="15.6">
       <c r="A105" s="2" t="s">
         <v>102</v>
       </c>
@@ -1886,7 +1900,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="106" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2" ht="15.6">
       <c r="A106" s="2" t="s">
         <v>103</v>
       </c>
@@ -1894,7 +1908,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="107" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2" ht="15.6">
       <c r="A107" s="2" t="s">
         <v>104</v>
       </c>
@@ -1902,7 +1916,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="108" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2" ht="15.6">
       <c r="A108" s="2" t="s">
         <v>105</v>
       </c>
@@ -1910,7 +1924,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="109" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" ht="15.6">
       <c r="A109" s="2" t="s">
         <v>106</v>
       </c>
@@ -1918,7 +1932,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="110" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" ht="15.6">
       <c r="A110" s="2" t="s">
         <v>107</v>
       </c>
@@ -1926,7 +1940,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="111" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:2" ht="15.6">
       <c r="A111" s="2" t="s">
         <v>108</v>
       </c>
@@ -1934,7 +1948,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="112" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:2" ht="15.6">
       <c r="A112" s="2" t="s">
         <v>109</v>
       </c>
@@ -1942,7 +1956,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="113" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:2" ht="15.6">
       <c r="A113" s="2" t="s">
         <v>110</v>
       </c>
@@ -1950,7 +1964,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="114" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:2" ht="15.6">
       <c r="A114" s="2" t="s">
         <v>111</v>
       </c>
@@ -1958,7 +1972,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="115" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:2" ht="15.6">
       <c r="A115" s="2" t="s">
         <v>112</v>
       </c>
@@ -1966,7 +1980,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="116" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:2" ht="15.6">
       <c r="A116" s="2" t="s">
         <v>113</v>
       </c>
@@ -1974,7 +1988,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="117" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:2" ht="15.6">
       <c r="A117" s="2" t="s">
         <v>114</v>
       </c>
@@ -1982,7 +1996,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="118" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:2" ht="15.6">
       <c r="A118" s="2" t="s">
         <v>115</v>
       </c>
@@ -1990,7 +2004,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="119" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:2" ht="15.6">
       <c r="A119" s="2" t="s">
         <v>116</v>
       </c>
@@ -1998,7 +2012,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="120" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:2" ht="15.6">
       <c r="A120" s="2" t="s">
         <v>117</v>
       </c>
@@ -2006,7 +2020,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="121" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:2" ht="15.6">
       <c r="A121" s="2" t="s">
         <v>118</v>
       </c>
@@ -2014,7 +2028,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="122" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:2" ht="15.6">
       <c r="A122" s="2" t="s">
         <v>119</v>
       </c>
@@ -2022,7 +2036,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="123" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:2" ht="15.6">
       <c r="A123" s="2" t="s">
         <v>120</v>
       </c>
@@ -2030,7 +2044,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="124" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:2" ht="15.6">
       <c r="A124" s="2" t="s">
         <v>121</v>
       </c>
@@ -2038,7 +2052,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="125" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:2" ht="15.6">
       <c r="A125" s="2" t="s">
         <v>122</v>
       </c>
@@ -2046,7 +2060,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="126" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:2" ht="15.6">
       <c r="A126" s="2" t="s">
         <v>123</v>
       </c>
@@ -2054,7 +2068,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="127" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:2" ht="15.6">
       <c r="A127" s="2" t="s">
         <v>124</v>
       </c>
@@ -2062,7 +2076,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="128" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:2" ht="15.6">
       <c r="A128" s="2" t="s">
         <v>125</v>
       </c>
@@ -2070,7 +2084,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="129" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:2" ht="15.6">
       <c r="A129" s="2" t="s">
         <v>126</v>
       </c>
@@ -2078,63 +2092,63 @@
         <v>4</v>
       </c>
     </row>
-    <row r="130" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:2" ht="15.6">
       <c r="A130" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B130" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" ht="15.6">
+      <c r="A131" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B130" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A131" s="2" t="s">
+      <c r="B131" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" ht="15.6">
+      <c r="A132" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="B131" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A132" s="2" t="s">
+      <c r="B132" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" ht="15.6">
+      <c r="A133" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B132" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A133" s="2" t="s">
+      <c r="B133" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" ht="15.6">
+      <c r="A134" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B133" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A134" s="2" t="s">
+      <c r="B134" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" ht="15.6">
+      <c r="A135" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="B134" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A135" s="2" t="s">
+      <c r="B135" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" ht="15.6">
+      <c r="A136" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="B135" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A136" s="2" t="s">
-        <v>133</v>
-      </c>
       <c r="B136" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="137" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:2" ht="15.6">
       <c r="A137" s="2" t="s">
         <v>28</v>
       </c>
@@ -2142,515 +2156,523 @@
         <v>3</v>
       </c>
     </row>
-    <row r="138" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:2" ht="15.6">
       <c r="A138" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B138" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" ht="15.6">
+      <c r="A139" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="B138" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A139" s="2" t="s">
+      <c r="B139" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" ht="15.6">
+      <c r="A140" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="B139" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A140" s="2" t="s">
+      <c r="B140" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" ht="15.6">
+      <c r="A141" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="B140" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A141" s="2" t="s">
+      <c r="B141" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" ht="15.6">
+      <c r="A142" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="B141" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A142" s="2" t="s">
+      <c r="B142" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" ht="15.6">
+      <c r="A143" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="B142" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A143" s="2" t="s">
+      <c r="B143" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" ht="15.6">
+      <c r="A144" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="B143" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A144" s="2" t="s">
+      <c r="B144" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" ht="15.6">
+      <c r="A145" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="B144" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A145" s="2" t="s">
+      <c r="B145" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" ht="15.6">
+      <c r="A146" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="B145" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A146" s="2" t="s">
+      <c r="B146" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" ht="15.6">
+      <c r="A147" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="B146" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A147" s="2" t="s">
+      <c r="B147" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" ht="15.6">
+      <c r="A148" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="B147" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A148" s="2" t="s">
+      <c r="B148" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" ht="15.6">
+      <c r="A149" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="B148" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A149" s="2" t="s">
+      <c r="B149" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" ht="15.6">
+      <c r="A150" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="B149" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A150" s="2" t="s">
+      <c r="B150" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" ht="15.6">
+      <c r="A151" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="B150" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A151" s="2" t="s">
+      <c r="B151" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" ht="15.6">
+      <c r="A152" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="B151" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A152" s="2" t="s">
+      <c r="B152" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" ht="15.6">
+      <c r="A153" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="B152" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A153" s="2" t="s">
+      <c r="B153" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" ht="15.6">
+      <c r="A154" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="B153" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A154" s="2" t="s">
+      <c r="B154" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" ht="15.6">
+      <c r="A155" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="B154" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="155" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A155" s="2" t="s">
+      <c r="B155" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" ht="15.6">
+      <c r="A156" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="B155" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="156" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A156" s="2" t="s">
+      <c r="B156" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" ht="15.6">
+      <c r="A157" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B156" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="157" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A157" s="2" t="s">
+      <c r="B157" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" ht="15.6">
+      <c r="A158" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="B157" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="158" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A158" s="2" t="s">
+      <c r="B158" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" ht="15.6">
+      <c r="A159" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="B158" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A159" s="2" t="s">
+      <c r="B159" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" ht="15.6">
+      <c r="A160" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B159" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="160" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A160" s="2" t="s">
+      <c r="B160" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" ht="15.6">
+      <c r="A161" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="B160" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="161" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A161" s="2" t="s">
+      <c r="B161" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" ht="15.6">
+      <c r="A162" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="B161" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="162" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A162" s="2" t="s">
+      <c r="B162" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" ht="15.6">
+      <c r="A163" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="B162" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="163" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A163" s="2" t="s">
+      <c r="B163" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" ht="15.6">
+      <c r="A164" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="B163" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="164" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A164" s="2" t="s">
+      <c r="B164" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" ht="15.6">
+      <c r="A165" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="B164" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="165" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A165" s="2" t="s">
+      <c r="B165" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" ht="15.6">
+      <c r="A166" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="B165" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="166" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A166" s="2" t="s">
+      <c r="B166" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" ht="15.6">
+      <c r="A167" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="B166" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="167" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A167" s="2" t="s">
+      <c r="B167" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" ht="15.6">
+      <c r="A168" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="B167" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="168" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A168" s="2" t="s">
+      <c r="B168" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" ht="15.6">
+      <c r="A169" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="B168" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="169" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A169" s="2" t="s">
+      <c r="B169" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" ht="15.6">
+      <c r="A170" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="B169" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="170" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A170" s="2" t="s">
+      <c r="B170" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" ht="15.6">
+      <c r="A171" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="B170" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="171" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A171" s="2" t="s">
+      <c r="B171" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" ht="15.6">
+      <c r="A172" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="B171" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="172" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A172" s="2" t="s">
+      <c r="B172" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" ht="15.6">
+      <c r="A173" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="B172" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="173" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A173" s="2" t="s">
+      <c r="B173" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" ht="15.6">
+      <c r="A174" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="B173" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="174" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A174" s="2" t="s">
+      <c r="B174" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" ht="15.6">
+      <c r="A175" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="B174" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="175" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A175" s="2" t="s">
+      <c r="B175" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" ht="15.6">
+      <c r="A176" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="B175" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="176" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A176" s="2" t="s">
+      <c r="B176" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" ht="15.6">
+      <c r="A177" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="B176" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="177" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A177" s="2" t="s">
+      <c r="B177" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" ht="15.6">
+      <c r="A178" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="B177" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="178" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A178" s="2" t="s">
+      <c r="B178" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" ht="15.6">
+      <c r="A179" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="B178" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="179" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A179" s="2" t="s">
+      <c r="B179" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" ht="15.6">
+      <c r="A180" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="B179" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="180" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A180" s="2" t="s">
+      <c r="B180" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" ht="15.6">
+      <c r="A181" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="B180" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="181" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A181" s="2" t="s">
+      <c r="B181" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" ht="15.6">
+      <c r="A182" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="B181" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="182" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A182" s="2" t="s">
+      <c r="B182" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" ht="15.6">
+      <c r="A183" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B183" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" ht="15.6">
+      <c r="A184" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="B182" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="183" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A183" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="B183" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="184" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A184" s="2" t="s">
+      <c r="B184" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" ht="15.6">
+      <c r="A185" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="B184" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="185" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A185" s="2" t="s">
+      <c r="B185" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" ht="15.6">
+      <c r="A186" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="B185" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="186" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A186" s="2" t="s">
+      <c r="B186" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" ht="15.6">
+      <c r="A187" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="B187" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" ht="15.6">
+      <c r="A188" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="B186" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="187" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A187" s="2" t="s">
+      <c r="B188" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" ht="15.6">
+      <c r="A189" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="B187" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="188" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A188" s="2" t="s">
+      <c r="B189" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" ht="15.6">
+      <c r="A190" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="B188" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="189" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A189" s="2" t="s">
+      <c r="B190" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" ht="15.6">
+      <c r="A191" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="B189" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="190" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A190" s="2" t="s">
+      <c r="B191" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" ht="15.6">
+      <c r="A192" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="B190" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="191" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A191" s="2" t="s">
+      <c r="B192" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" ht="15.6">
+      <c r="A193" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="B191" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="192" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A192" s="2" t="s">
+      <c r="B193" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" ht="15.6">
+      <c r="A194" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="B192" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="193" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A193" s="2" t="s">
+      <c r="B194" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" ht="15.6">
+      <c r="A195" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="B193" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="194" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A194" s="2" t="s">
+      <c r="B195" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" ht="15.6">
+      <c r="A196" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="B194" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="195" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A195" s="2" t="s">
+      <c r="B196" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" ht="15.6">
+      <c r="A197" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="B195" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="196" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A196" s="2" t="s">
+      <c r="B197" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" ht="15.6">
+      <c r="A198" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="B196" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="197" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A197" s="2" t="s">
+      <c r="B198" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" ht="15.6">
+      <c r="A199" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="B197" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="198" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A198" s="2" t="s">
+      <c r="B199" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" ht="15.6">
+      <c r="A200" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="B198" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="199" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A199" s="2" t="s">
+      <c r="B200" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" ht="15.6">
+      <c r="A201" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="B199" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="200" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A200" s="2" t="s">
+      <c r="B201" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" ht="15.6">
+      <c r="A202" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="B200" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="201" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A201" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="B201" s="4">
+      <c r="B202" s="4">
         <v>2</v>
       </c>
     </row>
@@ -2660,6 +2682,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5d0836d6-44f8-4bdc-b7ec-4ce50b8bd073">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="91634d5d-6728-474a-a339-016187646ac3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000F20F0DEBE5DAB4CB09FAD3571EFEFD3" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="156855e6115abbda6c28c215b288d477">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5d0836d6-44f8-4bdc-b7ec-4ce50b8bd073" xmlns:ns3="31cb4620-1988-46c0-a0bc-9ed88a7d10ff" xmlns:ns4="91634d5d-6728-474a-a339-016187646ac3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bc170a0dd204544c80e7fa01fa1049f2" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="5d0836d6-44f8-4bdc-b7ec-4ce50b8bd073"/>
@@ -2919,31 +2961,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5d0836d6-44f8-4bdc-b7ec-4ce50b8bd073">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="91634d5d-6728-474a-a339-016187646ac3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA0CE157-9AB4-40E4-88AE-48480C2B3938}"/>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{943F6530-DAE3-4EC0-814A-296BA57D35A5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -2951,7 +2969,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A290D032-9ED6-46FE-9312-EAB9C715F544}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -2964,6 +2982,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="5d0836d6-44f8-4bdc-b7ec-4ce50b8bd073"/>
+    <ds:schemaRef ds:uri="91634d5d-6728-474a-a339-016187646ac3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA0CE157-9AB4-40E4-88AE-48480C2B3938}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="5d0836d6-44f8-4bdc-b7ec-4ce50b8bd073"/>
+    <ds:schemaRef ds:uri="31cb4620-1988-46c0-a0bc-9ed88a7d10ff"/>
+    <ds:schemaRef ds:uri="91634d5d-6728-474a-a339-016187646ac3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>